<commit_message>
Update: Coa and extract
</commit_message>
<xml_diff>
--- a/out/errors.xlsx
+++ b/out/errors.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,6 +450,40 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>\\192.168.29.200\f\service\0.样品管理部\01 蛋白库相关\06 蛋白编号\00 理化质检-P90000之后在这里查理化质检结果\SEC</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>【SEC】WKL230904-1 ZJ004 HLX1005 HNKJ001.pptx</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>File is not a zip file</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>\\192.168.29.200\f\service\0.样品管理部\01 蛋白库相关\06 蛋白编号\00 理化质检-P90000之后在这里查理化质检结果\SEC</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>【SEC】WKL230904-1 ZJ004 HLX1005 HNKJ001.pdf</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NoRelatedPPT</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>